<commit_message>
update BOM, add comment.
</commit_message>
<xml_diff>
--- a/ATLink-Lite/HW/ATLink_v21.9.24_BOM.xlsx
+++ b/ATLink-Lite/HW/ATLink_v21.9.24_BOM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="106">
   <si>
     <t>Comment</t>
   </si>
@@ -572,13 +572,174 @@
       </rPr>
       <t>贴片晶振</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>备注</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>红色</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>LED</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>使用</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>4.7k</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>就足够亮了</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.5k</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>电阻不焊接</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>可更换为</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>10uF</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>，减少器件种类</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>默认不焊接</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>可焊接双排直针</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>0805 0.5A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>自恢复保险丝</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>SS8050</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>也可以</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -607,6 +768,19 @@
       <family val="2"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -622,7 +796,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -645,13 +819,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -662,6 +847,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -958,16 +1155,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="6" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -986,8 +1185,11 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1007,7 +1209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1026,8 +1228,11 @@
       <c r="F3" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -1047,7 +1252,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
@@ -1067,7 +1272,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -1087,7 +1292,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
@@ -1107,7 +1312,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
         <v>30</v>
       </c>
@@ -1126,8 +1331,11 @@
       <c r="F8" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
         <v>34</v>
       </c>
@@ -1147,7 +1355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:7">
       <c r="A10" s="2" t="s">
         <v>37</v>
       </c>
@@ -1166,8 +1374,11 @@
       <c r="F10" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="2" t="s">
         <v>88</v>
       </c>
@@ -1187,7 +1398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:7">
       <c r="A12" s="2" t="s">
         <v>44</v>
       </c>
@@ -1206,9 +1417,12 @@
       <c r="F12" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="2" t="s">
+      <c r="G12" s="6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="5" t="s">
         <v>48</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1226,8 +1440,11 @@
       <c r="F13" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="2" t="s">
         <v>52</v>
       </c>
@@ -1247,7 +1464,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:7">
       <c r="A15" s="2" t="s">
         <v>55</v>
       </c>
@@ -1266,8 +1483,11 @@
       <c r="F15" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="2" t="s">
         <v>58</v>
       </c>
@@ -1287,7 +1507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:7">
       <c r="A17" s="2" t="s">
         <v>61</v>
       </c>
@@ -1307,7 +1527,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:7">
       <c r="A18" s="2" t="s">
         <v>64</v>
       </c>
@@ -1327,8 +1547,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="2" t="s">
+    <row r="19" spans="1:7">
+      <c r="A19" s="5" t="s">
         <v>68</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -1346,8 +1566,11 @@
       <c r="F19" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="2" t="s">
         <v>71</v>
       </c>
@@ -1367,7 +1590,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:7">
       <c r="A21" s="2" t="s">
         <v>73</v>
       </c>
@@ -1387,7 +1610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:7">
       <c r="A22" s="2" t="s">
         <v>76</v>
       </c>
@@ -1407,7 +1630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:7">
       <c r="A23" s="2" t="s">
         <v>81</v>
       </c>

</xml_diff>